<commit_message>
added missing x for Raia initial conditions
</commit_message>
<xml_diff>
--- a/Benchmark-Models/benchmark_model_characteristics.xlsx
+++ b/Benchmark-Models/benchmark_model_characteristics.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28028"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2240" yWindow="-16580" windowWidth="25400" windowHeight="14520" tabRatio="500" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="2244" yWindow="-16584" windowWidth="23256" windowHeight="13176" tabRatio="500" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="model_characteristics" sheetId="1" r:id="rId1"/>
@@ -14,13 +14,10 @@
     <definedName name="colors" localSheetId="1">model_overview!$B$1:$E$22</definedName>
     <definedName name="colors_1" localSheetId="1">model_overview!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
@@ -921,300 +918,300 @@
     </xf>
   </cellXfs>
   <cellStyles count="295">
-    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="94" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="96" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="98" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="100" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="102" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="104" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="106" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="108" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="110" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="112" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="114" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="116" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="118" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="120" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="122" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="124" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="126" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="128" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="130" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="132" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="134" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="136" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="138" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="140" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="142" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="144" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="146" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="148" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="150" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="152" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="154" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="156" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="158" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="160" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="162" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="164" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="166" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="168" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="170" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="172" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="174" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="176" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="178" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="180" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="182" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="184" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="186" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="188" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="190" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="192" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="194" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="196" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="198" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="200" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="202" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="204" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="206" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="208" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="210" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="212" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="214" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="216" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="218" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="220" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="222" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="224" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="226" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="228" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="230" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="232" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="234" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="236" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="238" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="240" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="242" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="244" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="246" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="248" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="250" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="252" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="254" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="256" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="258" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="260" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="262" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="264" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="266" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="268" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="270" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="272" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="274" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="276" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="278" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="280" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="282" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="284" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="286" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="288" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="290" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="292" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="294" builtinId="9" hidden="1"/>
-    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="75" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="79" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="81" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="83" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="85" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="87" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="89" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="91" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="93" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="95" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="97" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="99" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="101" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="103" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="105" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="107" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="109" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="111" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="113" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="115" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="117" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="119" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="121" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="123" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="125" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="127" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="129" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="131" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="133" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="135" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="137" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="139" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="141" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="143" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="145" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="147" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="149" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="151" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="153" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="155" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="157" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="159" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="161" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="163" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="165" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="167" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="169" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="171" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="173" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="175" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="177" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="179" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="181" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="183" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="185" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="187" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="189" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="191" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="193" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="195" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="197" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="199" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="201" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="203" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="205" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="207" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="209" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="211" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="213" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="215" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="217" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="219" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="221" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="223" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="225" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="227" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="229" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="231" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="233" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="235" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="237" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="239" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="241" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="243" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="245" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="247" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="249" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="251" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="253" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="255" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="257" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="259" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="261" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="263" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="265" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="267" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="269" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="271" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="273" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="275" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="277" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="279" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="281" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="283" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="285" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="287" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="289" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="291" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="293" builtinId="8" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="262" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="264" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="266" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="280" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="282" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="284" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="286" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="288" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="275" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="277" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="279" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="293" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1230,7 +1227,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1336,7 +1333,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>299.00751503006</c:v>
+                  <c:v>299.00751503006001</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>101.7465</c:v>
@@ -1345,52 +1342,52 @@
                   <c:v>1357.29889298893</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>105.597</c:v>
+                  <c:v>105.59699999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>174.07835258664</c:v>
+                  <c:v>174.07835258663999</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>28.6295</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>723.90494296578</c:v>
+                  <c:v>723.90494296578004</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>214.209562563581</c:v>
+                  <c:v>214.20956256358099</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>34.7399732620321</c:v>
+                  <c:v>34.739973262032102</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>84.62391033623911</c:v>
+                  <c:v>84.623910336239106</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>139.172804532578</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>250.587112171838</c:v>
+                  <c:v>250.58711217183799</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>316.842105263158</c:v>
+                  <c:v>316.84210526315798</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>279.578</c:v>
+                  <c:v>279.57799999999997</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>174.166581762608</c:v>
+                  <c:v>174.16658176260799</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>210.489493201483</c:v>
+                  <c:v>210.48949320148299</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>146.421806853583</c:v>
+                  <c:v>146.42180685358301</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>342.277673545966</c:v>
+                  <c:v>342.27767354596602</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2170.0025</c:v>
+                  <c:v>2170.0025000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1406,11 +1403,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2095602280"/>
-        <c:axId val="2095602632"/>
+        <c:axId val="61605760"/>
+        <c:axId val="61607296"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2095602280"/>
+        <c:axId val="61605760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1450,10 +1447,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2095602632"/>
+        <c:crossAx val="61607296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1461,7 +1458,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2095602632"/>
+        <c:axId val="61607296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1544,10 +1541,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2095602280"/>
+        <c:crossAx val="61605760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1585,7 +1582,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1599,7 +1596,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1692,8 +1689,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.104811504671241"/>
-                  <c:y val="-0.0372464754000782"/>
+                  <c:x val="-0.10481150467124099"/>
+                  <c:y val="-3.7246475400078201E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1721,7 +1718,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="de-DE"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1738,58 +1735,58 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="20"/>
                   <c:pt idx="0">
-                    <c:v>3.88318392235657</c:v>
+                    <c:v>3.8831839223565701</c:v>
                   </c:pt>
                   <c:pt idx="1">
                     <c:v>1.5920370972044</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>55.3273843044006</c:v>
+                    <c:v>55.327384304400603</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>3.29602970185343</c:v>
+                    <c:v>3.2960297018534299</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>3.92151096761745</c:v>
+                    <c:v>3.9215109676174502</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0.233948957841236</c:v>
+                    <c:v>0.23394895784123601</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>17.0445677555079</c:v>
+                    <c:v>17.044567755507899</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>7.24378011238457</c:v>
+                    <c:v>7.2437801123845702</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>0.713182934392782</c:v>
+                    <c:v>0.71318293439278202</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>3.22605051328147</c:v>
+                    <c:v>3.2260505132814701</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>7.67404499693348</c:v>
+                    <c:v>7.6740449969334801</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>6.25939450352804</c:v>
+                    <c:v>6.2593945035280401</c:v>
                   </c:pt>
                   <c:pt idx="13">
-                    <c:v>5.50048543023543</c:v>
+                    <c:v>5.5004854302354298</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>4.88500736519404</c:v>
+                    <c:v>4.8850073651940402</c:v>
                   </c:pt>
                   <c:pt idx="15">
                     <c:v>2.46120869090988</c:v>
                   </c:pt>
                   <c:pt idx="16">
-                    <c:v>6.40946279561252</c:v>
+                    <c:v>6.4094627956125203</c:v>
                   </c:pt>
                   <c:pt idx="17">
-                    <c:v>4.8964050725793</c:v>
+                    <c:v>4.8964050725792996</c:v>
                   </c:pt>
                   <c:pt idx="18">
-                    <c:v>14.4487035049037</c:v>
+                    <c:v>14.448703504903699</c:v>
                   </c:pt>
                   <c:pt idx="19">
                     <c:v>34.9155404619042</c:v>
@@ -1804,58 +1801,58 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="20"/>
                   <c:pt idx="0">
-                    <c:v>3.88318392235657</c:v>
+                    <c:v>3.8831839223565701</c:v>
                   </c:pt>
                   <c:pt idx="1">
                     <c:v>1.5920370972044</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>55.3273843044006</c:v>
+                    <c:v>55.327384304400603</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>3.29602970185343</c:v>
+                    <c:v>3.2960297018534299</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>3.92151096761745</c:v>
+                    <c:v>3.9215109676174502</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0.233948957841236</c:v>
+                    <c:v>0.23394895784123601</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>17.0445677555079</c:v>
+                    <c:v>17.044567755507899</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>7.24378011238457</c:v>
+                    <c:v>7.2437801123845702</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>0.713182934392782</c:v>
+                    <c:v>0.71318293439278202</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>3.22605051328147</c:v>
+                    <c:v>3.2260505132814701</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>7.67404499693348</c:v>
+                    <c:v>7.6740449969334801</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>6.25939450352804</c:v>
+                    <c:v>6.2593945035280401</c:v>
                   </c:pt>
                   <c:pt idx="13">
-                    <c:v>5.50048543023543</c:v>
+                    <c:v>5.5004854302354298</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>4.88500736519404</c:v>
+                    <c:v>4.8850073651940402</c:v>
                   </c:pt>
                   <c:pt idx="15">
                     <c:v>2.46120869090988</c:v>
                   </c:pt>
                   <c:pt idx="16">
-                    <c:v>6.40946279561252</c:v>
+                    <c:v>6.4094627956125203</c:v>
                   </c:pt>
                   <c:pt idx="17">
-                    <c:v>4.8964050725793</c:v>
+                    <c:v>4.8964050725792996</c:v>
                   </c:pt>
                   <c:pt idx="18">
-                    <c:v>14.4487035049037</c:v>
+                    <c:v>14.448703504903699</c:v>
                   </c:pt>
                   <c:pt idx="19">
                     <c:v>34.9155404619042</c:v>
@@ -1882,7 +1879,7 @@
             <c:errBarType val="both"/>
             <c:errValType val="fixedVal"/>
             <c:noEndCap val="0"/>
-            <c:val val="1.0"/>
+            <c:val val="1"/>
             <c:spPr>
               <a:noFill/>
               <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -1904,64 +1901,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>113.0</c:v>
+                  <c:v>113</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>72.0</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>22.0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>191.0</c:v>
+                  <c:v>191</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>22.0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>22.0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>62.0</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>46.0</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>84.0</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>197.0</c:v>
+                  <c:v>197</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>39.0</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>269.0</c:v>
+                  <c:v>269</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>36.0</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>46.0</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1973,7 +1970,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>299.00751503006</c:v>
+                  <c:v>299.00751503006001</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>101.7465</c:v>
@@ -1982,52 +1979,52 @@
                   <c:v>1357.29889298893</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>105.597</c:v>
+                  <c:v>105.59699999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>174.07835258664</c:v>
+                  <c:v>174.07835258663999</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>28.6295</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>723.90494296578</c:v>
+                  <c:v>723.90494296578004</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>214.209562563581</c:v>
+                  <c:v>214.20956256358099</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>34.7399732620321</c:v>
+                  <c:v>34.739973262032102</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>84.62391033623911</c:v>
+                  <c:v>84.623910336239106</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>139.172804532578</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>250.587112171838</c:v>
+                  <c:v>250.58711217183799</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>316.842105263158</c:v>
+                  <c:v>316.84210526315798</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>279.578</c:v>
+                  <c:v>279.57799999999997</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>174.166581762608</c:v>
+                  <c:v>174.16658176260799</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>210.489493201483</c:v>
+                  <c:v>210.48949320148299</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>146.421806853583</c:v>
+                  <c:v>146.42180685358301</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>342.277673545966</c:v>
+                  <c:v>342.27767354596602</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2170.0025</c:v>
+                  <c:v>2170.0025000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2042,11 +2039,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2095648024"/>
-        <c:axId val="2095651032"/>
+        <c:axId val="61620992"/>
+        <c:axId val="61622528"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2095648024"/>
+        <c:axId val="61620992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2100,15 +2097,15 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2095651032"/>
+        <c:crossAx val="61622528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2095651032"/>
+        <c:axId val="61622528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2162,10 +2159,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2095648024"/>
+        <c:crossAx val="61620992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2203,7 +2200,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2217,7 +2214,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2266,64 +2263,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>113.0</c:v>
+                  <c:v>113</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>72.0</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>22.0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>191.0</c:v>
+                  <c:v>191</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>22.0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>22.0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>62.0</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>46.0</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>84.0</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>197.0</c:v>
+                  <c:v>197</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>39.0</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>269.0</c:v>
+                  <c:v>269</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>36.0</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>46.0</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2335,31 +2332,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2374,11 +2371,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2090316360"/>
-        <c:axId val="2090325208"/>
+        <c:axId val="61642240"/>
+        <c:axId val="61644800"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2090316360"/>
+        <c:axId val="61642240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2467,18 +2464,18 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2090325208"/>
+        <c:crossAx val="61644800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2090325208"/>
+        <c:axId val="61644800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1.0"/>
+          <c:max val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2565,13 +2562,13 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2090316360"/>
+        <c:crossAx val="61642240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="1.0"/>
+        <c:majorUnit val="1"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -2607,7 +2604,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4627,7 +4624,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4641,13 +4638,13 @@
       <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="13" max="13" width="6.1640625" customWidth="1"/>
-    <col min="14" max="15" width="13.6640625" customWidth="1"/>
+    <col min="13" max="13" width="6.19921875" customWidth="1"/>
+    <col min="14" max="15" width="13.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4697,7 +4694,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -4751,7 +4748,7 @@
         <v>0.20848708487084872</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -4802,7 +4799,7 @@
         <v>0.18823529411764706</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -4856,7 +4853,7 @@
         <v>2.6536930561698365E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -4907,7 +4904,7 @@
         <v>0.1875</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -4961,7 +4958,7 @@
         <v>0.51162790697674421</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -5012,7 +5009,7 @@
         <v>0.16883116883116883</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -5057,7 +5054,7 @@
         <v>1.819047619047619</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -5108,7 +5105,7 @@
         <v>0.76190476190476186</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -5159,7 +5156,7 @@
         <v>0.30555555555555558</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -5210,7 +5207,7 @@
         <v>0.15277777777777779</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -5264,7 +5261,7 @@
         <v>0.28054298642533937</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -5315,7 +5312,7 @@
         <v>6.4516129032258063E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -5369,7 +5366,7 @@
         <v>4.7863247863247867E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -5423,7 +5420,7 @@
         <v>0.1726555652936021</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -5474,7 +5471,7 @@
         <v>0.19024390243902439</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -5525,7 +5522,7 @@
         <v>0.10273972602739725</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -5579,7 +5576,7 @@
         <v>0.12117117117117117</v>
       </c>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -5630,7 +5627,7 @@
         <v>0.30434782608695654</v>
       </c>
     </row>
-    <row r="20" spans="1:17">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -5684,7 +5681,7 @@
         <v>0.26666666666666666</v>
       </c>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -5738,7 +5735,7 @@
         <v>0.76666666666666672</v>
       </c>
     </row>
-    <row r="24" spans="1:17">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D24" t="s">
         <v>30</v>
       </c>
@@ -5749,7 +5746,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D25">
         <v>0</v>
       </c>
@@ -5769,7 +5766,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D26">
         <v>1</v>
       </c>
@@ -5789,7 +5786,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:17">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D27">
         <v>2</v>
       </c>
@@ -5809,7 +5806,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:17">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="G28">
         <v>3</v>
       </c>
@@ -5840,23 +5837,23 @@
   <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="22"/>
-    <col min="2" max="2" width="28.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" style="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.1640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.796875" style="22"/>
+    <col min="2" max="2" width="28.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.296875" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.19921875" style="22" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.69921875" style="22" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.5" style="22" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="6" style="22" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.1640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.19921875" style="22" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="3.5" style="22" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="6" style="22" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8.5" style="22" bestFit="1" customWidth="1"/>
@@ -5864,11 +5861,11 @@
     <col min="16" max="16" width="6" style="22" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="8.5" style="22" bestFit="1" customWidth="1"/>
     <col min="18" max="20" width="3.5" style="22" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="190.33203125" style="22" customWidth="1"/>
-    <col min="22" max="16384" width="10.83203125" style="22"/>
+    <col min="21" max="21" width="190.296875" style="22" customWidth="1"/>
+    <col min="22" max="16384" width="10.796875" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" ht="32" customHeight="1">
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
@@ -5911,7 +5908,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="1" customFormat="1" ht="78">
+    <row r="2" spans="1:21" s="1" customFormat="1" ht="76.8" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
         <v>103</v>
       </c>
@@ -5966,7 +5963,7 @@
       </c>
       <c r="U2" s="6"/>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>51</v>
       </c>
@@ -6018,7 +6015,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>52</v>
       </c>
@@ -6070,7 +6067,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>53</v>
       </c>
@@ -6122,7 +6119,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>54</v>
       </c>
@@ -6174,7 +6171,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>55</v>
       </c>
@@ -6226,7 +6223,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="24" t="s">
         <v>56</v>
       </c>
@@ -6278,7 +6275,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>105</v>
       </c>
@@ -6330,7 +6327,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>57</v>
       </c>
@@ -6382,7 +6379,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>58</v>
       </c>
@@ -6434,7 +6431,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>59</v>
       </c>
@@ -6486,7 +6483,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>63</v>
       </c>
@@ -6538,7 +6535,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>60</v>
       </c>
@@ -6590,7 +6587,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>67</v>
       </c>
@@ -6642,7 +6639,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>61</v>
       </c>
@@ -6694,7 +6691,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="17" spans="1:21">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>62</v>
       </c>
@@ -6746,7 +6743,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:21">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>64</v>
       </c>
@@ -6798,7 +6795,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="1:21">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>65</v>
       </c>
@@ -6850,7 +6847,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="20" spans="1:21">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>66</v>
       </c>
@@ -6902,7 +6899,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:21">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>68</v>
       </c>
@@ -6954,7 +6951,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="1:21">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>69</v>
       </c>

</xml_diff>